<commit_message>
Update data files - Bot run at 2026-02-12 15:58:34 UTC
</commit_message>
<xml_diff>
--- a/dm_promotion_service/data/users_engagement.xlsx
+++ b/dm_promotion_service/data/users_engagement.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -736,6 +736,39 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1417827147</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>user_1417827147</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>unreachable</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Added during extraction</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>